<commit_message>
teta mathod work, but...
Нужно придумать пересчет V и L
V выводится без учета teta
</commit_message>
<xml_diff>
--- a/Черновик.xlsx
+++ b/Черновик.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D516EF43-60D6-43F3-BF5D-C0D852C6A038}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <sheet name="Лист10" sheetId="10" r:id="rId10"/>
     <sheet name="Лист2" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -610,13 +611,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
     <numFmt numFmtId="166" formatCode="0.000000000"/>
     <numFmt numFmtId="167" formatCode="0.00000000000"/>
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -829,14 +830,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -855,7 +856,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -1003,7 +1004,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B3D3-4661-AB45-63880700E643}"/>
             </c:ext>
@@ -1138,7 +1139,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-B3D3-4661-AB45-63880700E643}"/>
             </c:ext>
@@ -1273,7 +1274,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-B3D3-4661-AB45-63880700E643}"/>
             </c:ext>
@@ -1457,14 +1458,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1500,7 +1501,7 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -1595,7 +1596,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8F06-40CA-B413-6C07B89771C5}"/>
             </c:ext>
@@ -1667,7 +1668,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8F06-40CA-B413-6C07B89771C5}"/>
             </c:ext>
@@ -1739,7 +1740,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-8F06-40CA-B413-6C07B89771C5}"/>
             </c:ext>
@@ -1867,7 +1868,7 @@
 </file>
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -1949,7 +1950,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-46D6-4870-89F9-59CD719C989F}"/>
             </c:ext>
@@ -2018,7 +2019,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-46D6-4870-89F9-59CD719C989F}"/>
             </c:ext>
@@ -2085,7 +2086,7 @@
 </file>
 
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -2180,7 +2181,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-001B-4440-A1AC-8572DEF38482}"/>
             </c:ext>
@@ -2252,7 +2253,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-001B-4440-A1AC-8572DEF38482}"/>
             </c:ext>
@@ -2324,7 +2325,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-001B-4440-A1AC-8572DEF38482}"/>
             </c:ext>
@@ -2450,7 +2451,7 @@
 </file>
 
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -2545,7 +2546,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A45C-4D14-8A36-0BAEB0B4315C}"/>
             </c:ext>
@@ -2617,7 +2618,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-A45C-4D14-8A36-0BAEB0B4315C}"/>
             </c:ext>
@@ -2689,7 +2690,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-A45C-4D14-8A36-0BAEB0B4315C}"/>
             </c:ext>
@@ -2815,7 +2816,7 @@
 </file>
 
 <file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -2910,7 +2911,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A45C-4D14-8A36-0BAEB0B4315C}"/>
             </c:ext>
@@ -3034,7 +3035,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3116,7 +3117,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-06BC-4342-9122-CF435FB8F99C}"/>
             </c:ext>
@@ -3185,7 +3186,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-06BC-4342-9122-CF435FB8F99C}"/>
             </c:ext>
@@ -3237,7 +3238,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3253,7 +3253,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3335,7 +3335,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8382-4CF4-BACD-692918FE94EF}"/>
             </c:ext>
@@ -3404,7 +3404,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8382-4CF4-BACD-692918FE94EF}"/>
             </c:ext>
@@ -3471,7 +3471,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3553,7 +3553,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7B6A-4222-9C4F-10E6AD2F7FAC}"/>
             </c:ext>
@@ -3622,7 +3622,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7B6A-4222-9C4F-10E6AD2F7FAC}"/>
             </c:ext>
@@ -3689,7 +3689,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3771,7 +3771,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9A94-4C66-9C18-15CF3E93214B}"/>
             </c:ext>
@@ -3840,7 +3840,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9A94-4C66-9C18-15CF3E93214B}"/>
             </c:ext>
@@ -3907,7 +3907,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3989,7 +3989,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C17C-4D74-93EA-1ED41F7C0803}"/>
             </c:ext>
@@ -4058,7 +4058,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C17C-4D74-93EA-1ED41F7C0803}"/>
             </c:ext>
@@ -4125,7 +4125,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -4207,7 +4207,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-91C6-4B38-8F28-2CCB79346E5E}"/>
             </c:ext>
@@ -4276,7 +4276,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-91C6-4B38-8F28-2CCB79346E5E}"/>
             </c:ext>
@@ -4343,7 +4343,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -4425,7 +4425,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2223-4EFB-B12D-E467CC54C56E}"/>
             </c:ext>
@@ -4494,7 +4494,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2223-4EFB-B12D-E467CC54C56E}"/>
             </c:ext>
@@ -4561,7 +4561,7 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -4643,7 +4643,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3FA5-4024-A456-3BB79B9F971B}"/>
             </c:ext>
@@ -4712,7 +4712,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-3FA5-4024-A456-3BB79B9F971B}"/>
             </c:ext>
@@ -5354,7 +5354,7 @@
         <xdr:cNvPr id="2" name="Диаграмма 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1376E361-9B03-4C46-9E16-696541727A54}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1376E361-9B03-4C46-9E16-696541727A54}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5395,7 +5395,7 @@
         <xdr:cNvPr id="2" name="Диаграмма 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5431,7 +5431,7 @@
         <xdr:cNvPr id="3" name="Диаграмма 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5469,7 +5469,7 @@
         <xdr:cNvPr id="4" name="Диаграмма 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5505,7 +5505,7 @@
         <xdr:cNvPr id="5" name="Диаграмма 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5541,7 +5541,7 @@
         <xdr:cNvPr id="6" name="Диаграмма 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D69D8E43-BE20-4D14-A4F1-21A80679D980}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D69D8E43-BE20-4D14-A4F1-21A80679D980}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5582,7 +5582,7 @@
         <xdr:cNvPr id="2" name="Диаграмма 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5623,7 +5623,7 @@
         <xdr:cNvPr id="2" name="Диаграмма 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5666,7 +5666,7 @@
         <xdr:cNvPr id="2" name="Диаграмма 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5709,7 +5709,7 @@
         <xdr:cNvPr id="2" name="Диаграмма 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5752,7 +5752,7 @@
         <xdr:cNvPr id="2" name="Диаграмма 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5795,7 +5795,7 @@
         <xdr:cNvPr id="2" name="Диаграмма 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5838,7 +5838,7 @@
         <xdr:cNvPr id="2" name="Диаграмма 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5881,7 +5881,7 @@
         <xdr:cNvPr id="2" name="Диаграмма 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0800-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6159,14 +6159,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6867,7 +6867,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:S117"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -8649,17 +8649,17 @@
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="32" t="s">
+      <c r="A95" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B95" s="33" t="s">
+      <c r="B95" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="C95" s="33"/>
-      <c r="D95" s="33"/>
+      <c r="C95" s="35"/>
+      <c r="D95" s="35"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="32"/>
+      <c r="A96" s="34"/>
       <c r="B96" s="18" t="s">
         <v>70</v>
       </c>
@@ -8776,17 +8776,17 @@
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="32" t="s">
+      <c r="A103" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B103" s="33" t="s">
+      <c r="B103" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="C103" s="33"/>
-      <c r="D103" s="33"/>
+      <c r="C103" s="35"/>
+      <c r="D103" s="35"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="32"/>
+      <c r="A104" s="34"/>
       <c r="B104" s="18" t="s">
         <v>70</v>
       </c>
@@ -8883,17 +8883,17 @@
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="32" t="s">
+      <c r="A111" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B111" s="33" t="s">
+      <c r="B111" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="C111" s="33"/>
-      <c r="D111" s="33"/>
+      <c r="C111" s="35"/>
+      <c r="D111" s="35"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="32"/>
+      <c r="A112" s="34"/>
       <c r="B112" s="18" t="s">
         <v>70</v>
       </c>
@@ -9002,7 +9002,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A2:K39"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -9905,37 +9905,37 @@
       <c r="A30">
         <v>13.8</v>
       </c>
-      <c r="B30" s="34">
+      <c r="B30" s="32">
         <v>2.2222222222222199E-2</v>
       </c>
-      <c r="C30" s="35">
+      <c r="C30" s="33">
         <f>B30*$A$30</f>
         <v>0.30666666666666637</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="34">
+      <c r="B31" s="32">
         <v>4.4444444444444398E-2</v>
       </c>
-      <c r="C31" s="35">
+      <c r="C31" s="33">
         <f t="shared" ref="C31:C38" si="4">B31*$A$30</f>
         <v>0.61333333333333273</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="34">
+      <c r="B32" s="32">
         <v>6.6666666666666693E-2</v>
       </c>
-      <c r="C32" s="35">
+      <c r="C32" s="33">
         <f t="shared" si="4"/>
         <v>0.92000000000000037</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="34">
+      <c r="B33" s="32">
         <v>8.8888888888888906E-2</v>
       </c>
-      <c r="C33" s="35">
+      <c r="C33" s="33">
         <f t="shared" si="4"/>
         <v>1.226666666666667</v>
       </c>
@@ -9944,7 +9944,7 @@
       <c r="B34">
         <v>0.11111111111111099</v>
       </c>
-      <c r="C34" s="35">
+      <c r="C34" s="33">
         <f t="shared" si="4"/>
         <v>1.5333333333333319</v>
       </c>
@@ -9953,7 +9953,7 @@
       <c r="B35">
         <v>0.133333333333333</v>
       </c>
-      <c r="C35" s="35">
+      <c r="C35" s="33">
         <f t="shared" si="4"/>
         <v>1.8399999999999954</v>
       </c>
@@ -9962,7 +9962,7 @@
       <c r="B36">
         <v>0.155555555555556</v>
       </c>
-      <c r="C36" s="35">
+      <c r="C36" s="33">
         <f t="shared" si="4"/>
         <v>2.1466666666666727</v>
       </c>
@@ -9971,7 +9971,7 @@
       <c r="B37">
         <v>0.17777777777777801</v>
       </c>
-      <c r="C37" s="35">
+      <c r="C37" s="33">
         <f t="shared" si="4"/>
         <v>2.4533333333333367</v>
       </c>
@@ -9980,13 +9980,13 @@
       <c r="B38">
         <v>0.2</v>
       </c>
-      <c r="C38" s="35">
+      <c r="C38" s="33">
         <f t="shared" si="4"/>
         <v>2.7600000000000002</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C39" s="35"/>
+      <c r="C39" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9994,10 +9994,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
@@ -11739,7 +11739,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S87"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
@@ -13505,7 +13505,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S87"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
@@ -15270,7 +15270,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S87"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
@@ -17036,7 +17036,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:S87"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
@@ -18801,7 +18801,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:S87"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -20566,7 +20566,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:S87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22331,7 +22331,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:S87"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">

</xml_diff>